<commit_message>
Feature: Version 1.1 Enthaltene Änderungen in dieser Version: - [Bugfix] Button auf der Startseite war nicht verlinkt ("Über") - [Feature] Spalte "Edition" hinzugefügt (etwa Standard, Limited oder Best-Of-Ausgaben wie "Platinum-Edition") - [Feature] Seite "Hilfe und Info" angelegt - [Feature] Zubehör-Schema als Vorschlag hinzugefügt (Für die Spalte "Zubehör", siehe "Hilfe und Info") - [Improvement] Kleine Anpassungen am Design, den Abständen und Zell-Ausrichtungen - [Feature] Weitere Beispiel-Games hinzugefügt
</commit_message>
<xml_diff>
--- a/pixelpommes Retro-Game-Collection.xlsx
+++ b/pixelpommes Retro-Game-Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karsten/Desktop/Retro-Sammlung-Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32F38FF-0979-9E41-ACED-BA45B43494C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6119E3-E545-D84A-A7D9-D1F55621EEB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" xr2:uid="{9B36302A-304C-ED4B-9F14-A525393D165C}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="Games" sheetId="3" r:id="rId2"/>
     <sheet name="Game-Cards drucken" sheetId="7" r:id="rId3"/>
     <sheet name="Game-Cards (Template)" sheetId="5" r:id="rId4"/>
-    <sheet name="Intern" sheetId="6" r:id="rId5"/>
+    <sheet name="Hilfe und Info" sheetId="8" r:id="rId5"/>
+    <sheet name="Intern" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="card_id_1">'Game-Cards drucken'!$E$18</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="133">
   <si>
     <t>pixelpommes Retro-Sammlung</t>
   </si>
@@ -109,9 +110,6 @@
     <t>Dieses Blatt ist für interne Werte im Programm gedacht, die an anderer Stelle verwendet werden.</t>
   </si>
   <si>
-    <t>In aller Regel muss hier nichts geändert werden!</t>
-  </si>
-  <si>
     <t>Statistik</t>
   </si>
   <si>
@@ -136,9 +134,6 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>Aktionen</t>
   </si>
   <si>
@@ -262,10 +257,31 @@
     <t>Google (EAN)</t>
   </si>
   <si>
+    <t>Mortal Kombat 11</t>
+  </si>
+  <si>
+    <t>Mortal Kombat</t>
+  </si>
+  <si>
+    <t>5051890317735</t>
+  </si>
+  <si>
     <t>Neuwertig</t>
   </si>
   <si>
-    <t>Super Mario</t>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Street Fighter</t>
+  </si>
+  <si>
+    <t>0045496420574</t>
+  </si>
+  <si>
+    <t>Street Fighter 30th Anniversary Collection</t>
+  </si>
+  <si>
+    <t>5055060948415</t>
   </si>
   <si>
     <t>Card gedruckt</t>
@@ -274,28 +290,166 @@
     <t>x</t>
   </si>
   <si>
+    <t>Zelda</t>
+  </si>
+  <si>
+    <t>0045496420093</t>
+  </si>
+  <si>
+    <t>Stern Pinball Arcade</t>
+  </si>
+  <si>
+    <t>Stern Pinball</t>
+  </si>
+  <si>
+    <t>5060057024652</t>
+  </si>
+  <si>
     <t>Doom</t>
   </si>
   <si>
-    <t>Super Mario Land</t>
-  </si>
-  <si>
-    <t>1234567</t>
-  </si>
-  <si>
-    <t>Gebraucht</t>
-  </si>
-  <si>
-    <t>Trödelmarkt</t>
-  </si>
-  <si>
-    <t>456789</t>
-  </si>
-  <si>
-    <t>Komplett</t>
+    <t>0045496421359</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Hilfe und Info</t>
+  </si>
+  <si>
+    <t>Abkürzungen (Zubehör)</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Box (Papp- oder Bigbox)</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Inlay</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Disk (Cartridge oder CD / DVD / BD / Diskette)</t>
+  </si>
+  <si>
+    <t>Case (Standard-Hülle)</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>C I D</t>
+  </si>
+  <si>
+    <t>Beim PS2-Kauf enthalten</t>
+  </si>
+  <si>
+    <t>GTA Vice City</t>
+  </si>
+  <si>
+    <t>GTA</t>
+  </si>
+  <si>
+    <t>Ausgabe</t>
+  </si>
+  <si>
+    <t>Platinum Edition</t>
+  </si>
+  <si>
+    <t>C I D E</t>
+  </si>
+  <si>
+    <t>Gebraucht (CD hat Gebrauchsspuren)</t>
+  </si>
+  <si>
+    <t>Extras (Etwa eine Karte, weiteres Produkt innerhalb der Box oder Case)</t>
+  </si>
+  <si>
+    <t>Tekken 5</t>
+  </si>
+  <si>
+    <t>Tekken</t>
+  </si>
+  <si>
+    <t>0711719637264</t>
+  </si>
+  <si>
+    <t>Gebraucht (Leichte Gebrauchsspuren)</t>
   </si>
   <si>
     <t>eBay</t>
+  </si>
+  <si>
+    <t>GTA San Andreas</t>
+  </si>
+  <si>
+    <t>5026555302630</t>
+  </si>
+  <si>
+    <t>Tekken 4</t>
+  </si>
+  <si>
+    <t>0711719619710</t>
+  </si>
+  <si>
+    <t>Neuwertig (Hülle Gebraucht)</t>
+  </si>
+  <si>
+    <t>C D</t>
+  </si>
+  <si>
+    <t>Über</t>
+  </si>
+  <si>
+    <t>Informationen</t>
+  </si>
+  <si>
+    <t>Jeder Gaming-Begeisterte verwaltet seine Sammlung anders. Ich habe mit dieser Vorlage versucht, ein möglichst einfaches und übersichtliches</t>
+  </si>
+  <si>
+    <t>Inventar für meine Game-Sammlung anzulegen. Viele von euch werden sicherlich weitere Features wie Einkaufspreise etc. inventarisieren wollen.</t>
+  </si>
+  <si>
+    <t>Daher ist diese Datei auch nur eine Vorlage, die jeder gerne an seine Bedürfnisse anpassen kann.</t>
+  </si>
+  <si>
+    <t>Hinweis: Wenn ihr weitere Spalten anlegen wollt, empfehle ich, dies zwischen Spalte M und N zu tun, da ihr ansonsten die Spalten-Indexe</t>
+  </si>
+  <si>
+    <t>in den Game-Cards aktualisieren müsst (in den SVERWEIS-Funktionen). Das ist kein Problem, allerdings etwas nervig.</t>
+  </si>
+  <si>
+    <t>kombiniere ich einfach die Buchstaben und erhalte somit eine gute Angabe über alles, was enthalten ist. Ihr könnt natürlich auch jedes andere, beliebige</t>
+  </si>
+  <si>
+    <t>System verwenden.</t>
+  </si>
+  <si>
+    <t>Viel Spaß beim Sammeln und Inventarisieren!</t>
+  </si>
+  <si>
+    <t>Die Abkürzungen (oben rechts in diesem Blatt) sind mein persönliches Schema für die Angabe des Zubehörs. Wie ihr in der Zubehör-Spalte sehen könnt,</t>
+  </si>
+  <si>
+    <t>Hinweis: Pull-Requests auf GitHub werden nicht angenommen, ihr könnt euch aber gerne jederzeit mit Featurewünschen und Bug-Requests melden!</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>The Legend of Zelda - Breath of the Wild</t>
+  </si>
+  <si>
+    <t>Ultra Street Fighter II - The Final Challengers</t>
+  </si>
+  <si>
+    <t>In aller Regel muss hier nichts geändert werden, mit Ausnahme neuer Plattformen!</t>
   </si>
 </sst>
 </file>
@@ -705,7 +859,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -780,6 +934,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="4" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -789,6 +946,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
@@ -847,7 +1039,7 @@
     <cellStyle name="Tabellen_Zelle" xfId="6" xr:uid="{F64937A1-A3E9-6442-BFB1-BDECC2787485}"/>
     <cellStyle name="Textfeld" xfId="7" xr:uid="{5E92B938-5405-D845-8818-7F03312F1427}"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -906,6 +1098,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -922,6 +1115,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -930,6 +1124,17 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -939,6 +1144,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1032,9 +1238,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="pixelpommes" pivot="0" count="3" xr9:uid="{CB5C7279-C698-4D46-8DBC-60D60B4ACF98}">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1194,7 +1400,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1725,16 +1931,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -3134,6 +3340,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="Rechteck 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC252EAA-523B-CF4F-8302-16243172AE84}"/>
@@ -3221,7 +3428,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3259,7 +3466,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3346,16 +3553,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEC8CE58-CAC2-B646-BFA6-56B1E10D858B}" name="gamelist" displayName="gamelist" ref="B5:P7" totalsRowShown="0" dataDxfId="15" headerRowCellStyle="Tabellen_Headline">
-  <autoFilter ref="B5:P7" xr:uid="{E0F78244-26A4-1544-86B7-53AB99206D2A}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{91647493-BDCE-8B47-A24E-1EF8A2271C45}" name="ID" dataDxfId="14" dataCellStyle="Tabellen_Zelle">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEC8CE58-CAC2-B646-BFA6-56B1E10D858B}" name="gamelist" displayName="gamelist" ref="B5:Q15" totalsRowShown="0" dataDxfId="16" headerRowCellStyle="Tabellen_Headline">
+  <autoFilter ref="B5:Q15" xr:uid="{E0F78244-26A4-1544-86B7-53AB99206D2A}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{91647493-BDCE-8B47-A24E-1EF8A2271C45}" name="ID" dataDxfId="15" dataCellStyle="Tabellen_Zelle">
       <calculatedColumnFormula>ROW() - 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A242BAF9-7080-7A4D-8A14-4A673ED3F0BD}" name="Name" dataDxfId="13" dataCellStyle="Tabellen_Zelle"/>
-    <tableColumn id="3" xr3:uid="{B00F4DA3-AB3B-094D-A205-8FFA1E6DBEE9}" name="Franchise" dataDxfId="12" dataCellStyle="Tabellen_Zelle"/>
-    <tableColumn id="4" xr3:uid="{B8AC0DB0-4188-3A49-94C3-85E50363D2BF}" name="Plattform" dataDxfId="11" dataCellStyle="Tabellen_Zelle"/>
-    <tableColumn id="5" xr3:uid="{5A3E12B0-A448-914D-BE2B-B0BFC3B56167}" name="EAN (etc.)" dataDxfId="10" dataCellStyle="Tabellen_Zelle"/>
+    <tableColumn id="2" xr3:uid="{A242BAF9-7080-7A4D-8A14-4A673ED3F0BD}" name="Name" dataDxfId="14" dataCellStyle="Tabellen_Zelle"/>
+    <tableColumn id="3" xr3:uid="{B00F4DA3-AB3B-094D-A205-8FFA1E6DBEE9}" name="Franchise" dataDxfId="13" dataCellStyle="Tabellen_Zelle"/>
+    <tableColumn id="4" xr3:uid="{B8AC0DB0-4188-3A49-94C3-85E50363D2BF}" name="Plattform" dataDxfId="12" dataCellStyle="Tabellen_Zelle"/>
+    <tableColumn id="5" xr3:uid="{5A3E12B0-A448-914D-BE2B-B0BFC3B56167}" name="EAN (etc.)" dataDxfId="11" dataCellStyle="Tabellen_Zelle"/>
+    <tableColumn id="16" xr3:uid="{23BEA912-30AD-D64B-87B0-AB07FD3E3443}" name="Ausgabe" dataDxfId="10" dataCellStyle="Tabellen_Zelle"/>
     <tableColumn id="6" xr3:uid="{1303E69F-FC87-914B-8126-EFBD417E794A}" name="Zustand" dataDxfId="9" dataCellStyle="Tabellen_Zelle"/>
     <tableColumn id="7" xr3:uid="{70DBC594-45EC-DD48-AE45-2C5D71E5B48D}" name="Zubehör / Ausstattung" dataDxfId="8" dataCellStyle="Tabellen_Zelle"/>
     <tableColumn id="8" xr3:uid="{5A948789-4854-8149-9D57-58D1E8866392}" name="Quelle" dataDxfId="7" dataCellStyle="Tabellen_Zelle"/>
@@ -3679,7 +3887,7 @@
   <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3717,7 +3925,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
@@ -3753,7 +3961,7 @@
     <row r="6" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -3770,7 +3978,7 @@
       <c r="B7" s="15"/>
       <c r="C7" s="16" t="str">
         <f xml:space="preserve"> "Du benutzt die pixelpommes Retro-Sammlung in Version " &amp; programm_version</f>
-        <v>Du benutzt die pixelpommes Retro-Sammlung in Version 1.0</v>
+        <v>Du benutzt die pixelpommes Retro-Sammlung in Version 1.1</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -3787,7 +3995,7 @@
       <c r="B8" s="15"/>
       <c r="C8" s="16" t="str">
         <f>"Aktuell werden " &amp; game_anzahl &amp; " Games verwaltet."</f>
-        <v>Aktuell werden 2 Games verwaltet.</v>
+        <v>Aktuell werden 10 Games verwaltet.</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -3817,7 +4025,7 @@
     <row r="10" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -3889,7 +4097,7 @@
     <row r="15" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -4095,40 +4303,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D3F3F5-F0D3-4B44-BD42-F1B12C603E35}">
-  <dimension ref="B1:P7"/>
+  <dimension ref="B1:Q15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.7109375" style="1"/>
+    <col min="6" max="6" width="16.28515625" style="54" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4138,16 +4347,17 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="2:17" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -4157,14 +4367,15 @@
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="2:16" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="2:17" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="57"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -4174,9 +4385,10 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
-    </row>
-    <row r="5" spans="2:16" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="10"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="2:17" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
         <v>2</v>
       </c>
@@ -4189,135 +4401,526 @@
       <c r="E5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="58" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="I5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="J5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="K5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="L5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="28" t="s">
-        <v>72</v>
-      </c>
       <c r="M5" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="N5" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="28" t="s">
+      <c r="P5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="Q5" s="28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30">
         <f t="shared" ref="B6" si="0">ROW() - 5</f>
         <v>1</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D6" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="29" t="str">
-        <f t="shared" ref="M6:M7" si="1">HYPERLINK((google_prefix &amp; C6), "Öffnen")</f>
+      <c r="I6" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="29" t="str">
+        <f t="shared" ref="N6:N11" si="1">HYPERLINK((google_prefix &amp; C6), "Öffnen")</f>
         <v>Öffnen</v>
       </c>
-      <c r="N6" s="29" t="str">
-        <f t="shared" ref="N6:N7" si="2">HYPERLINK((google_prefix &amp; F6), "Öffnen")</f>
+      <c r="O6" s="29" t="str">
+        <f t="shared" ref="O6:O11" si="2">HYPERLINK((google_prefix &amp; F6), "Öffnen")</f>
         <v>Öffnen</v>
       </c>
-      <c r="O6" s="29" t="str">
-        <f t="shared" ref="O6:O7" si="3">HYPERLINK((mobygames_prefix &amp; C6), "Öffnen")</f>
+      <c r="P6" s="29" t="str">
+        <f t="shared" ref="P6:P11" si="3">HYPERLINK((mobygames_prefix &amp; C6), "Öffnen")</f>
         <v>Öffnen</v>
       </c>
-      <c r="P6" s="29" t="str">
-        <f t="shared" ref="P6:P7" si="4">HYPERLINK(mobygames_prefix_ean &amp; " " &amp;F6, "Öffnen")</f>
+      <c r="Q6" s="29" t="str">
+        <f t="shared" ref="Q6:Q11" si="4">HYPERLINK(mobygames_prefix_ean &amp; " " &amp;F6, "Öffnen")</f>
         <v>Öffnen</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30">
         <f t="shared" ref="B7" si="5">ROW() - 5</f>
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="M7" s="29" t="str">
+      <c r="G7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="29" t="str">
         <f t="shared" si="1"/>
         <v>Öffnen</v>
       </c>
-      <c r="N7" s="29" t="str">
+      <c r="O7" s="29" t="str">
         <f t="shared" si="2"/>
         <v>Öffnen</v>
       </c>
-      <c r="O7" s="29" t="str">
+      <c r="P7" s="29" t="str">
         <f t="shared" si="3"/>
         <v>Öffnen</v>
       </c>
-      <c r="P7" s="29" t="str">
+      <c r="Q7" s="29" t="str">
         <f t="shared" si="4"/>
         <v>Öffnen</v>
       </c>
     </row>
+    <row r="8" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="30">
+        <f t="shared" ref="B8:B11" si="6">ROW() - 5</f>
+        <v>3</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O8" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P8" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q8" s="29" t="str">
+        <f t="shared" si="4"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="30">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O9" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P9" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q9" s="29" t="str">
+        <f t="shared" si="4"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O10" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P10" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q10" s="29" t="str">
+        <f t="shared" si="4"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="30">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O11" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P11" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q11" s="29" t="str">
+        <f t="shared" si="4"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="30">
+        <f t="shared" ref="B12:B15" si="7">ROW() - 5</f>
+        <v>7</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="59"/>
+      <c r="G12" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="K12" s="32"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="29" t="str">
+        <f t="shared" ref="N12:N15" si="8">HYPERLINK((google_prefix &amp; C12), "Öffnen")</f>
+        <v>Öffnen</v>
+      </c>
+      <c r="O12" s="29" t="str">
+        <f t="shared" ref="O12:O15" si="9">HYPERLINK((google_prefix &amp; F12), "Öffnen")</f>
+        <v>Öffnen</v>
+      </c>
+      <c r="P12" s="29" t="str">
+        <f t="shared" ref="P12:P15" si="10">HYPERLINK((mobygames_prefix &amp; C12), "Öffnen")</f>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q12" s="29" t="str">
+        <f t="shared" ref="Q12:Q15" si="11">HYPERLINK(mobygames_prefix_ean &amp; " " &amp;F12, "Öffnen")</f>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="K13" s="32"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="29" t="str">
+        <f t="shared" si="8"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O13" s="29" t="str">
+        <f t="shared" si="9"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P13" s="29" t="str">
+        <f t="shared" si="10"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q13" s="29" t="str">
+        <f t="shared" si="11"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" s="32"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="29" t="str">
+        <f t="shared" si="8"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O14" s="29" t="str">
+        <f t="shared" si="9"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P14" s="29" t="str">
+        <f t="shared" si="10"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q14" s="29" t="str">
+        <f t="shared" si="11"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="30">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="32"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="29" t="str">
+        <f t="shared" si="8"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="O15" s="29" t="str">
+        <f t="shared" si="9"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="P15" s="29" t="str">
+        <f t="shared" si="10"/>
+        <v>Öffnen</v>
+      </c>
+      <c r="Q15" s="29" t="str">
+        <f t="shared" si="11"/>
+        <v>Öffnen</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="L6:L7">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="M6:M15">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4327,12 +4930,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7073C961-1064-6A44-A657-7DE05DCC740E}">
           <x14:formula1>
             <xm:f>Intern!$I$10:$I$23</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E7</xm:sqref>
+          <xm:sqref>E6:E15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4345,7 +4948,7 @@
   <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4373,7 +4976,7 @@
     <row r="3" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4383,7 +4986,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
@@ -4419,7 +5022,7 @@
     <row r="6" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -4435,7 +5038,7 @@
     <row r="7" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -4451,7 +5054,7 @@
     <row r="8" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -4481,7 +5084,7 @@
     <row r="10" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -4497,7 +5100,7 @@
     <row r="11" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -4513,7 +5116,7 @@
     <row r="12" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -4543,7 +5146,7 @@
     <row r="14" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -4559,7 +5162,7 @@
     <row r="15" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -4575,7 +5178,7 @@
     <row r="16" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -4606,14 +5209,14 @@
       <c r="B18" s="15"/>
       <c r="C18" s="24"/>
       <c r="D18" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="27">
         <v>1</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H18" s="27">
         <v>2</v>
@@ -4640,17 +5243,17 @@
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E20" s="27">
         <v>3</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H20" s="27">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
@@ -4674,14 +5277,14 @@
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
       <c r="D22" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E22" s="27">
         <v>5</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H22" s="27">
         <v>6</v>
@@ -4707,7 +5310,7 @@
     <row r="24" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -4814,16 +5417,16 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="63" t="str">
         <f>VLOOKUP(C2,gamelist[],2)</f>
-        <v>Super Mario Land</v>
-      </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="57" t="str">
+        <v>Mortal Kombat 11</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="73" t="str">
         <f>VLOOKUP(E2,gamelist[],2)</f>
-        <v>Doom</v>
-      </c>
-      <c r="E3" s="48"/>
+        <v>Ultra Street Fighter II - The Final Challengers</v>
+      </c>
+      <c r="E3" s="64"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -4842,18 +5445,18 @@
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="str">
         <f>VLOOKUP(C2,gamelist[],3)</f>
-        <v>Super Mario</v>
+        <v>Mortal Kombat</v>
       </c>
       <c r="C5" s="38">
-        <f>VLOOKUP(C2,gamelist[],9)</f>
+        <f>VLOOKUP(C2,gamelist[],10)</f>
         <v>0</v>
       </c>
       <c r="D5" s="41" t="str">
         <f>VLOOKUP(E2,gamelist[],3)</f>
-        <v>Doom</v>
+        <v>Street Fighter</v>
       </c>
       <c r="E5" s="38">
-        <f>VLOOKUP(E2,gamelist[],9)</f>
+        <f>VLOOKUP(E2,gamelist[],10)</f>
         <v>0</v>
       </c>
     </row>
@@ -4874,86 +5477,86 @@
     <row r="7" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="37" t="str">
         <f>VLOOKUP(C2,gamelist[],5)</f>
-        <v>1234567</v>
-      </c>
-      <c r="C7" s="38" t="str">
-        <f>VLOOKUP(C2,gamelist[],8)</f>
-        <v>Trödelmarkt</v>
+        <v>5051890317735</v>
+      </c>
+      <c r="C7" s="38">
+        <f>VLOOKUP(C2,gamelist[],9)</f>
+        <v>0</v>
       </c>
       <c r="D7" s="41" t="str">
         <f>VLOOKUP(E2,gamelist[],5)</f>
-        <v>456789</v>
-      </c>
-      <c r="E7" s="38" t="str">
+        <v>0045496420574</v>
+      </c>
+      <c r="E7" s="38">
+        <f>VLOOKUP(E2,gamelist[],9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="62"/>
+      <c r="D8" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="62"/>
+    </row>
+    <row r="9" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="69" t="str">
+        <f>VLOOKUP(C2,gamelist[],7)</f>
+        <v>Neuwertig</v>
+      </c>
+      <c r="C9" s="70"/>
+      <c r="D9" s="74" t="str">
+        <f>VLOOKUP(E2,gamelist[],7)</f>
+        <v>Neuwertig</v>
+      </c>
+      <c r="E9" s="70"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="62"/>
+    </row>
+    <row r="11" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="65" t="str">
+        <f>VLOOKUP(C2,gamelist[],8)</f>
+        <v>C D</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="75" t="str">
         <f>VLOOKUP(E2,gamelist[],8)</f>
-        <v>eBay</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="46"/>
-    </row>
-    <row r="9" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="str">
-        <f>VLOOKUP(C2,gamelist[],6)</f>
-        <v>Gebraucht</v>
-      </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="58" t="str">
-        <f>VLOOKUP(E2,gamelist[],6)</f>
-        <v>Neuwertig</v>
-      </c>
-      <c r="E9" s="54"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="46"/>
-    </row>
-    <row r="11" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49">
-        <f>VLOOKUP(C2,gamelist[],7)</f>
+        <v>C D</v>
+      </c>
+      <c r="E11" s="66"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="62"/>
+      <c r="D12" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="62"/>
+    </row>
+    <row r="13" spans="2:5" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="67">
+        <f>VLOOKUP(C2,gamelist[],11)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="59" t="str">
-        <f>VLOOKUP(E2,gamelist[],7)</f>
-        <v>Komplett</v>
-      </c>
-      <c r="E11" s="50"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="46"/>
-    </row>
-    <row r="13" spans="2:5" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51">
-        <f>VLOOKUP(C2,gamelist[],10)</f>
+      <c r="C13" s="68"/>
+      <c r="D13" s="72">
+        <f>VLOOKUP(E2,gamelist[],11)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="56">
-        <f>VLOOKUP(E2,gamelist[],10)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="52"/>
+      <c r="E13" s="68"/>
     </row>
     <row r="14" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="33" t="s">
@@ -4968,20 +5571,20 @@
       </c>
       <c r="E14" s="34">
         <f>card_id_4</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="str">
+      <c r="B15" s="63" t="str">
         <f>VLOOKUP(C14,gamelist[],2)</f>
-        <v>Doom</v>
-      </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="57" t="str">
+        <v>Street Fighter 30th Anniversary Collection</v>
+      </c>
+      <c r="C15" s="64"/>
+      <c r="D15" s="73" t="str">
         <f>VLOOKUP(E14,gamelist[],2)</f>
-        <v>Doom</v>
-      </c>
-      <c r="E15" s="48"/>
+        <v>GTA San Andreas</v>
+      </c>
+      <c r="E15" s="64"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
@@ -5000,18 +5603,18 @@
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="37" t="str">
         <f>VLOOKUP(C14,gamelist[],3)</f>
-        <v>Doom</v>
+        <v>Street Fighter</v>
       </c>
       <c r="C17" s="38">
-        <f>VLOOKUP(C14,gamelist[],9)</f>
+        <f>VLOOKUP(C14,gamelist[],10)</f>
         <v>0</v>
       </c>
       <c r="D17" s="41" t="str">
         <f>VLOOKUP(E14,gamelist[],3)</f>
-        <v>Doom</v>
+        <v>GTA</v>
       </c>
       <c r="E17" s="38">
-        <f>VLOOKUP(E14,gamelist[],9)</f>
+        <f>VLOOKUP(E14,gamelist[],10)</f>
         <v>0</v>
       </c>
     </row>
@@ -5032,86 +5635,86 @@
     <row r="19" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="str">
         <f>VLOOKUP(C14,gamelist[],5)</f>
-        <v>456789</v>
-      </c>
-      <c r="C19" s="38" t="str">
-        <f>VLOOKUP(C14,gamelist[],8)</f>
-        <v>eBay</v>
+        <v>5055060948415</v>
+      </c>
+      <c r="C19" s="38">
+        <f>VLOOKUP(C14,gamelist[],9)</f>
+        <v>0</v>
       </c>
       <c r="D19" s="41" t="str">
         <f>VLOOKUP(E14,gamelist[],5)</f>
-        <v>456789</v>
+        <v>5026555302630</v>
       </c>
       <c r="E19" s="38" t="str">
+        <f>VLOOKUP(E14,gamelist[],9)</f>
+        <v>Beim PS2-Kauf enthalten</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="62"/>
+    </row>
+    <row r="21" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="69" t="str">
+        <f>VLOOKUP(C14,gamelist[],7)</f>
+        <v>Neuwertig</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="74" t="str">
+        <f>VLOOKUP(E14,gamelist[],7)</f>
+        <v>Gebraucht (CD hat Gebrauchsspuren)</v>
+      </c>
+      <c r="E21" s="70"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="62"/>
+      <c r="D22" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="62"/>
+    </row>
+    <row r="23" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="65" t="str">
+        <f>VLOOKUP(C14,gamelist[],8)</f>
+        <v>C D</v>
+      </c>
+      <c r="C23" s="66"/>
+      <c r="D23" s="75" t="str">
         <f>VLOOKUP(E14,gamelist[],8)</f>
-        <v>eBay</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="46"/>
-    </row>
-    <row r="21" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="53" t="str">
-        <f>VLOOKUP(C14,gamelist[],6)</f>
-        <v>Neuwertig</v>
-      </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="58" t="str">
-        <f>VLOOKUP(E14,gamelist[],6)</f>
-        <v>Neuwertig</v>
-      </c>
-      <c r="E21" s="54"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="46"/>
-    </row>
-    <row r="23" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="49" t="str">
-        <f>VLOOKUP(C14,gamelist[],7)</f>
-        <v>Komplett</v>
-      </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="59" t="str">
-        <f>VLOOKUP(E14,gamelist[],7)</f>
-        <v>Komplett</v>
-      </c>
-      <c r="E23" s="50"/>
+        <v>C I D E</v>
+      </c>
+      <c r="E23" s="66"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="46"/>
-      <c r="D24" s="55" t="s">
+      <c r="C24" s="62"/>
+      <c r="D24" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="46"/>
+      <c r="E24" s="62"/>
     </row>
     <row r="25" spans="2:5" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="51">
-        <f>VLOOKUP(C14,gamelist[],10)</f>
+      <c r="B25" s="67">
+        <f>VLOOKUP(C14,gamelist[],11)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="56">
-        <f>VLOOKUP(E14,gamelist[],10)</f>
+      <c r="C25" s="68"/>
+      <c r="D25" s="72">
+        <f>VLOOKUP(E14,gamelist[],11)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="52"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="33" t="s">
@@ -5130,16 +5733,16 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="47" t="str">
+      <c r="B27" s="63" t="str">
         <f>VLOOKUP(C26,gamelist[],2)</f>
-        <v>Doom</v>
-      </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="57" t="str">
+        <v>Stern Pinball Arcade</v>
+      </c>
+      <c r="C27" s="64"/>
+      <c r="D27" s="73" t="str">
         <f>VLOOKUP(E26,gamelist[],2)</f>
         <v>Doom</v>
       </c>
-      <c r="E27" s="48"/>
+      <c r="E27" s="64"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="35" t="s">
@@ -5158,10 +5761,10 @@
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="37" t="str">
         <f>VLOOKUP(C26,gamelist[],3)</f>
-        <v>Doom</v>
+        <v>Stern Pinball</v>
       </c>
       <c r="C29" s="38">
-        <f>VLOOKUP(C26,gamelist[],9)</f>
+        <f>VLOOKUP(C26,gamelist[],10)</f>
         <v>0</v>
       </c>
       <c r="D29" s="41" t="str">
@@ -5169,7 +5772,7 @@
         <v>Doom</v>
       </c>
       <c r="E29" s="38">
-        <f>VLOOKUP(E26,gamelist[],9)</f>
+        <f>VLOOKUP(E26,gamelist[],10)</f>
         <v>0</v>
       </c>
     </row>
@@ -5190,86 +5793,86 @@
     <row r="31" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="37" t="str">
         <f>VLOOKUP(C26,gamelist[],5)</f>
-        <v>456789</v>
-      </c>
-      <c r="C31" s="38" t="str">
-        <f>VLOOKUP(C26,gamelist[],8)</f>
-        <v>eBay</v>
+        <v>5060057024652</v>
+      </c>
+      <c r="C31" s="38">
+        <f>VLOOKUP(C26,gamelist[],9)</f>
+        <v>0</v>
       </c>
       <c r="D31" s="41" t="str">
         <f>VLOOKUP(E26,gamelist[],5)</f>
-        <v>456789</v>
-      </c>
-      <c r="E31" s="38" t="str">
+        <v>0045496421359</v>
+      </c>
+      <c r="E31" s="38">
+        <f>VLOOKUP(E26,gamelist[],9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="62"/>
+      <c r="D32" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="62"/>
+    </row>
+    <row r="33" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="69" t="str">
+        <f>VLOOKUP(C26,gamelist[],7)</f>
+        <v>Neuwertig</v>
+      </c>
+      <c r="C33" s="70"/>
+      <c r="D33" s="74" t="str">
+        <f>VLOOKUP(E26,gamelist[],7)</f>
+        <v>Neuwertig</v>
+      </c>
+      <c r="E33" s="70"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="62"/>
+      <c r="D34" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="62"/>
+    </row>
+    <row r="35" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="65" t="str">
+        <f>VLOOKUP(C26,gamelist[],8)</f>
+        <v>C D</v>
+      </c>
+      <c r="C35" s="66"/>
+      <c r="D35" s="75" t="str">
         <f>VLOOKUP(E26,gamelist[],8)</f>
-        <v>eBay</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="46"/>
-    </row>
-    <row r="33" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="53" t="str">
-        <f>VLOOKUP(C26,gamelist[],6)</f>
-        <v>Neuwertig</v>
-      </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="58" t="str">
-        <f>VLOOKUP(E26,gamelist[],6)</f>
-        <v>Neuwertig</v>
-      </c>
-      <c r="E33" s="54"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="46"/>
-    </row>
-    <row r="35" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="49" t="str">
-        <f>VLOOKUP(C26,gamelist[],7)</f>
-        <v>Komplett</v>
-      </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="59" t="str">
-        <f>VLOOKUP(E26,gamelist[],7)</f>
-        <v>Komplett</v>
-      </c>
-      <c r="E35" s="50"/>
+        <v>C D</v>
+      </c>
+      <c r="E35" s="66"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="55" t="s">
+      <c r="C36" s="62"/>
+      <c r="D36" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="46"/>
+      <c r="E36" s="62"/>
     </row>
     <row r="37" spans="2:5" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="51">
-        <f>VLOOKUP(C26,gamelist[],10)</f>
+      <c r="B37" s="67">
+        <f>VLOOKUP(C26,gamelist[],11)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="56">
-        <f>VLOOKUP(E26,gamelist[],10)</f>
+      <c r="C37" s="68"/>
+      <c r="D37" s="72">
+        <f>VLOOKUP(E26,gamelist[],11)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="52"/>
+      <c r="E37" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="42">
@@ -5322,11 +5925,418 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B78ED4-A609-3949-9B55-695C598E37DC}">
+  <dimension ref="B1:K28"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1"/>
+    <col min="5" max="5" width="4.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="2:11" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="51"/>
+      <c r="E6" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="51" t="str">
+        <f xml:space="preserve"> "pixelpommes Retro-Collection " &amp; programm_version</f>
+        <v>pixelpommes Retro-Collection 1.1</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="48"/>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="51"/>
+      <c r="E8" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="51"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="17"/>
+    </row>
+    <row r="21" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="52"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="17"/>
+    </row>
+    <row r="24" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="17"/>
+    </row>
+    <row r="25" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="52"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="17"/>
+    </row>
+    <row r="26" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="17"/>
+    </row>
+    <row r="27" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="17"/>
+    </row>
+    <row r="28" spans="2:11" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="20"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{B9F0F772-D686-7840-A728-87522261EC98}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15EB355-B9D5-E042-A325-174467514724}">
   <dimension ref="B1:M30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5417,7 +6427,7 @@
     <row r="7" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" s="16" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -5447,20 +6457,20 @@
     <row r="9" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="C9" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
@@ -5469,18 +6479,18 @@
     <row r="10" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="16">
         <f>COUNTA(gamelist[Name])</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="G10" s="60" t="s">
+        <v>129</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16" t="s">
@@ -5497,7 +6507,7 @@
     <row r="11" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="16">
         <f>COUNTA(gamelist[Archiviert])</f>
@@ -5508,7 +6518,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J11" s="16">
         <f>COUNTIF(gamelist[Plattform], I11)</f>
@@ -5521,18 +6531,18 @@
     <row r="12" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="16">
         <f>COUNTIF(gamelist[Archiviert], "")</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J12" s="16">
         <f>COUNTIF(gamelist[Plattform], I12)</f>
@@ -5551,7 +6561,7 @@
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J13" s="16">
         <f>COUNTIF(gamelist[Plattform], I13)</f>
@@ -5564,7 +6574,7 @@
     <row r="14" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="16"/>
@@ -5572,7 +6582,7 @@
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J14" s="16">
         <f>COUNTIF(gamelist[Plattform], I14)</f>
@@ -5585,21 +6595,21 @@
     <row r="15" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="43" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>64</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J15" s="16">
         <f>COUNTIF(gamelist[Plattform], I15)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
@@ -5608,21 +6618,21 @@
     <row r="16" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>64</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J16" s="16">
         <f>COUNTIF(gamelist[Plattform], I16)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
@@ -5631,21 +6641,21 @@
     <row r="17" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>63</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J17" s="16">
         <f>COUNTIF(gamelist[Plattform], I17)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
@@ -5654,17 +6664,17 @@
     <row r="18" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="44"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J18" s="16">
         <f>COUNTIF(gamelist[Plattform], I18)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
@@ -5673,13 +6683,13 @@
     <row r="19" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="44"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J19" s="16">
         <f>COUNTIF(gamelist[Plattform], I19)</f>
@@ -5692,13 +6702,13 @@
     <row r="20" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="44"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J20" s="16">
         <f>COUNTIF(gamelist[Plattform], I20)</f>
@@ -5717,7 +6727,7 @@
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J21" s="16">
         <f>COUNTIF(gamelist[Plattform], I21)</f>
@@ -5736,7 +6746,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J22" s="16">
         <f>COUNTIF(gamelist[Plattform], I22)</f>
@@ -5755,7 +6765,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J23" s="16">
         <f>COUNTIF(gamelist[Plattform], I23)</f>

</xml_diff>